<commit_message>
Animal Kill added. Wolf able to Feast. Readonly Fields Added.
</commit_message>
<xml_diff>
--- a/Documents/ColorCodes.xlsx
+++ b/Documents/ColorCodes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Random</t>
   </si>
@@ -94,6 +94,39 @@
   </si>
   <si>
     <t>0008FF</t>
+  </si>
+  <si>
+    <t>Gans</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>macht einen Satz nach vorn</t>
+  </si>
+  <si>
+    <t>Rollt sich zusammen</t>
+  </si>
+  <si>
+    <t>läuft schlangenlinien</t>
+  </si>
+  <si>
+    <t>Wechselt die lane</t>
+  </si>
+  <si>
+    <t>Ist manchmal giftig</t>
+  </si>
+  <si>
+    <t>wirft Stöcke</t>
+  </si>
+  <si>
+    <t>legt eier</t>
+  </si>
+  <si>
+    <t>Nur bei Währung</t>
+  </si>
+  <si>
+    <t>Löcher</t>
   </si>
 </sst>
 </file>
@@ -545,15 +578,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D19"/>
+  <dimension ref="C2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -561,115 +597,149 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>